<commit_message>
credit memo, invoice, prepayments
</commit_message>
<xml_diff>
--- a/templates/QARSF/SYDATA.xlsx
+++ b/templates/QARSF/SYDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\WS_RSAutomation\rsqasampleproj\templates\QARSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C0B875-9997-4615-AA43-720687457DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2477D825-7DA0-48C2-96CF-71F52280457F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="761" firstSheet="31" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -47,6 +47,7 @@
     <sheet name="ReopenInvoiceBatch" sheetId="30" r:id="rId32"/>
     <sheet name="CloseInvoiceBatch" sheetId="31" r:id="rId33"/>
     <sheet name="TransferInvoiceBatch" sheetId="32" r:id="rId34"/>
+    <sheet name="PrepaymentReleaseRecall" sheetId="39" r:id="rId35"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="80">
   <si>
     <t>API Mode</t>
   </si>
@@ -268,6 +269,45 @@
   </si>
   <si>
     <t>Sales Order Payment Cancel Authorization</t>
+  </si>
+  <si>
+    <t>CustomerNumber</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>ApplicationAvailability</t>
+  </si>
+  <si>
+    <t>ApplicationMethod</t>
+  </si>
+  <si>
+    <t>Cust-Dollar WF1 (8)</t>
+  </si>
+  <si>
+    <t>Maximum Amount</t>
+  </si>
+  <si>
+    <t>Prepayment Release</t>
+  </si>
+  <si>
+    <t>Prepayment Recall</t>
+  </si>
+  <si>
+    <t>Transaction Type Recall</t>
+  </si>
+  <si>
+    <t>Background Processing Recall</t>
+  </si>
+  <si>
+    <t>Transaction Type CloseOut</t>
+  </si>
+  <si>
+    <t>Background Processing CloseOut</t>
+  </si>
+  <si>
+    <t>Prepayment Close Out</t>
   </si>
 </sst>
 </file>
@@ -617,7 +657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
@@ -1841,7 +1881,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,7 +1980,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,6 +2008,97 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502F24E3-35CE-4D20-B93D-E042852331C2}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="https://rstk-qa-rsf.my.salesforce.com/a6J1K000000Qgsa" xr:uid="{5CFEA579-4305-4DF5-9B14-3A7B7B35261C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>